<commit_message>
Sent img names from backend to frontend
</commit_message>
<xml_diff>
--- a/backend/app/data/DellaBellaGeography.xlsx
+++ b/backend/app/data/DellaBellaGeography.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alyssa/Documents/GitHub/playing-cards/backend/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB40B897-38E4-0640-B6A7-CA3997138D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC58A9C-BB33-2440-ABB3-6379DBF55FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17560" windowHeight="16460" xr2:uid="{7F5CDC5C-C3A2-A647-988B-30F25FFDF368}"/>
+    <workbookView xWindow="13280" yWindow="520" windowWidth="17560" windowHeight="16460" xr2:uid="{7F5CDC5C-C3A2-A647-988B-30F25FFDF368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,12 +556,12 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -1189,7 +1189,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>43</v>

</xml_diff>